<commit_message>
Changes to experimental results
</commit_message>
<xml_diff>
--- a/experimental_results.xlsx
+++ b/experimental_results.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="11">
   <si>
     <t>Path length</t>
   </si>
@@ -64,9 +63,6 @@
   </si>
   <si>
     <t>P = 49</t>
-  </si>
-  <si>
-    <t>P = 89</t>
   </si>
 </sst>
 </file>
@@ -442,11 +438,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="190574928"/>
-        <c:axId val="190563424"/>
+        <c:axId val="-637376576"/>
+        <c:axId val="-595169552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190574928"/>
+        <c:axId val="-637376576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190563424"/>
+        <c:crossAx val="-595169552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -553,7 +549,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190563424"/>
+        <c:axId val="-595169552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,7 +663,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190574928"/>
+        <c:crossAx val="-637376576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1071,11 +1067,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="319590384"/>
-        <c:axId val="319592160"/>
+        <c:axId val="-594462096"/>
+        <c:axId val="-594457936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="319590384"/>
+        <c:axId val="-594462096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1170,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319592160"/>
+        <c:crossAx val="-594457936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1182,7 +1178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319592160"/>
+        <c:axId val="-594457936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,7 +1289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319590384"/>
+        <c:crossAx val="-594462096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4301,7 +4297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
@@ -5843,7 +5839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
       <selection activeCell="S50" sqref="S50"/>
     </sheetView>
   </sheetViews>
@@ -7385,7 +7381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
@@ -8920,597 +8916,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H79"/>
-  <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>5</v>
-      </c>
-      <c r="C1">
-        <v>5</v>
-      </c>
-      <c r="D1">
-        <v>5</v>
-      </c>
-      <c r="E1">
-        <v>5</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>15</v>
-      </c>
-      <c r="C17">
-        <v>15</v>
-      </c>
-      <c r="D17">
-        <v>15</v>
-      </c>
-      <c r="E17">
-        <v>15</v>
-      </c>
-      <c r="F17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>20</v>
-      </c>
-      <c r="C25">
-        <v>20</v>
-      </c>
-      <c r="D25">
-        <v>20</v>
-      </c>
-      <c r="E25">
-        <v>20</v>
-      </c>
-      <c r="F25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33">
-        <v>25</v>
-      </c>
-      <c r="C33">
-        <v>25</v>
-      </c>
-      <c r="D33">
-        <v>25</v>
-      </c>
-      <c r="E33">
-        <v>25</v>
-      </c>
-      <c r="F33">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41">
-        <v>30</v>
-      </c>
-      <c r="C41">
-        <v>30</v>
-      </c>
-      <c r="D41">
-        <v>30</v>
-      </c>
-      <c r="E41">
-        <v>30</v>
-      </c>
-      <c r="F41">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49">
-        <v>35</v>
-      </c>
-      <c r="C49">
-        <v>35</v>
-      </c>
-      <c r="D49">
-        <v>35</v>
-      </c>
-      <c r="E49">
-        <v>35</v>
-      </c>
-      <c r="F49">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57">
-        <v>40</v>
-      </c>
-      <c r="C57">
-        <v>40</v>
-      </c>
-      <c r="D57">
-        <v>40</v>
-      </c>
-      <c r="E57">
-        <v>40</v>
-      </c>
-      <c r="F57">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65">
-        <v>45</v>
-      </c>
-      <c r="C65">
-        <v>45</v>
-      </c>
-      <c r="D65">
-        <v>45</v>
-      </c>
-      <c r="E65">
-        <v>45</v>
-      </c>
-      <c r="F65">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73">
-        <v>50</v>
-      </c>
-      <c r="C73">
-        <v>50</v>
-      </c>
-      <c r="D73">
-        <v>50</v>
-      </c>
-      <c r="E73">
-        <v>50</v>
-      </c>
-      <c r="F73">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>5</v>
-      </c>
-      <c r="B74">
-        <v>100</v>
-      </c>
-      <c r="C74">
-        <v>100</v>
-      </c>
-      <c r="D74">
-        <v>100</v>
-      </c>
-      <c r="E74">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75">
-        <v>57</v>
-      </c>
-      <c r="C75">
-        <v>47</v>
-      </c>
-      <c r="D75">
-        <v>39</v>
-      </c>
-      <c r="E75">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="C76">
-        <v>0.47</v>
-      </c>
-      <c r="D76">
-        <v>0.39</v>
-      </c>
-      <c r="E76">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>1</v>
-      </c>
-      <c r="B77">
-        <v>0</v>
-      </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-      <c r="D78">
-        <v>7</v>
-      </c>
-      <c r="E78">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>4</v>
-      </c>
-      <c r="B79">
-        <v>32</v>
-      </c>
-      <c r="C79">
-        <v>34</v>
-      </c>
-      <c r="D79">
-        <v>25</v>
-      </c>
-      <c r="E79">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>